<commit_message>
Update Mobile No added
</commit_message>
<xml_diff>
--- a/PfcAPI/FileUploaded/SampleUpdatedata.xlsx
+++ b/PfcAPI/FileUploaded/SampleUpdatedata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Candidate ID</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Updated Name</t>
+  </si>
+  <si>
+    <t>Updated Phone No</t>
+  </si>
+  <si>
+    <t>9038655199</t>
   </si>
 </sst>
 </file>
@@ -68,17 +74,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -113,20 +127,23 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
-  <tableColumns count="3">
-    <tableColumn id="2" name="Candidate ID" dataDxfId="2"/>
-    <tableColumn id="1" name="Updated Name" dataDxfId="1"/>
-    <tableColumn id="4" name="Updated Date Of Joining" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:D2">
+    <filterColumn colId="3"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="2" name="Candidate ID" dataDxfId="5"/>
+    <tableColumn id="1" name="Updated Name" dataDxfId="4"/>
+    <tableColumn id="4" name="Updated Date Of Joining" dataDxfId="3"/>
+    <tableColumn id="3" name="Updated Phone No" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,20 +434,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -440,8 +459,11 @@
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -450,6 +472,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>